<commit_message>
Consulta ao Facebook Insights e Exibição no Dashboard Streamlit
</commit_message>
<xml_diff>
--- a/data/sp24/raw/Anúncios-SP24-.xlsx
+++ b/data/sp24/raw/Anúncios-SP24-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="66">
   <si>
     <t>Dia</t>
   </si>
@@ -74,6 +74,21 @@
     <t>Término dos relatórios</t>
   </si>
   <si>
+    <t>2024-02-22</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2024-02-21</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-19</t>
+  </si>
+  <si>
     <t>2024-02-18</t>
   </si>
   <si>
@@ -90,9 +105,6 @@
   </si>
   <si>
     <t>2024-02-13</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>2024-02-12</t>
@@ -538,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -634,55 +646,55 @@
         <v>20</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>968.38</v>
+        <v>358.44</v>
       </c>
       <c r="C2" s="6" t="n">
-        <v>69454.0</v>
+        <v>20474.0</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>13.94275348</v>
+        <v>17.50708215</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>33998.0</v>
+        <v>13639.0</v>
       </c>
       <c r="F2" s="7" t="n">
-        <v>28.4834402</v>
+        <v>26.2805191</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>2.04288488</v>
+        <v>1.50113645</v>
       </c>
       <c r="H2" s="7" t="n">
-        <v>179.0</v>
+        <v>64.0</v>
       </c>
       <c r="I2" s="7" t="n">
-        <v>5.40994413</v>
+        <v>5.600625</v>
       </c>
       <c r="J2" s="7" t="n">
-        <v>0.25772454</v>
+        <v>0.31259158</v>
       </c>
       <c r="K2" s="7" t="n">
-        <v>107.0</v>
+        <v>39.0</v>
       </c>
       <c r="L2" s="7" t="n">
-        <v>9.05028037</v>
+        <v>9.19076923</v>
       </c>
       <c r="M2" s="7" t="n">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="N2" s="7" t="n">
-        <v>121.0475</v>
-      </c>
-      <c r="O2" s="7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="P2" s="7" t="n">
-        <v>322.79333333</v>
-      </c>
-      <c r="Q2" s="7" t="n">
-        <v>4274.25</v>
-      </c>
-      <c r="R2" s="7" t="n">
-        <v>4.41381482</v>
+        <v>358.44</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="S2" s="8" t="s">
         <v>20</v>
@@ -693,312 +705,312 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>1526.13</v>
+        <v>1590.53</v>
       </c>
       <c r="C3" s="6" t="n">
-        <v>93253.0</v>
+        <v>89303.0</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>16.36547886</v>
+        <v>17.81048789</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>39210.0</v>
+        <v>35877.0</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>38.92195868</v>
+        <v>44.33285949</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>2.37829635</v>
+        <v>2.48914346</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>241.0</v>
+        <v>239.0</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>6.33248963</v>
+        <v>6.65493724</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>0.25843673</v>
+        <v>0.26762819</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>165.0</v>
+        <v>173.0</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>9.24927273</v>
+        <v>9.19381503</v>
       </c>
       <c r="M3" s="7" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
       <c r="N3" s="7" t="n">
-        <v>508.71</v>
+        <v>122.34846154</v>
       </c>
       <c r="O3" s="7" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="P3" s="7" t="n">
-        <v>381.5325</v>
+        <v>795.265</v>
       </c>
       <c r="Q3" s="7" t="n">
-        <v>3468.66</v>
+        <v>6950.87</v>
       </c>
       <c r="R3" s="7" t="n">
-        <v>2.27284701</v>
+        <v>4.37015963</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>1531.39</v>
+        <v>1609.3</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>94191.0</v>
+        <v>91590.0</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>16.2583474</v>
+        <v>17.57069549</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>43048.0</v>
+        <v>34440.0</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>35.57401041</v>
+        <v>46.72764228</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>2.1880459</v>
+        <v>2.65940767</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>268.0</v>
+        <v>211.0</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>5.71414179</v>
+        <v>7.62701422</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>0.28452825</v>
+        <v>0.2303745</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>197.0</v>
+        <v>144.0</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>7.7735533</v>
+        <v>11.17569444</v>
       </c>
       <c r="M4" s="7" t="n">
-        <v>32.0</v>
+        <v>12.0</v>
       </c>
       <c r="N4" s="7" t="n">
-        <v>47.8559375</v>
+        <v>134.10833333</v>
       </c>
       <c r="O4" s="7" t="n">
-        <v>12.0</v>
+        <v>7.0</v>
       </c>
       <c r="P4" s="7" t="n">
-        <v>127.61583333</v>
+        <v>229.9</v>
       </c>
       <c r="Q4" s="7" t="n">
-        <v>5732.79</v>
+        <v>13432.53</v>
       </c>
       <c r="R4" s="7" t="n">
-        <v>3.74352059</v>
+        <v>8.34681539</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>1560.39</v>
+        <v>1657.51</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>92473.0</v>
+        <v>98819.0</v>
       </c>
       <c r="D5" s="7" t="n">
-        <v>16.87400647</v>
+        <v>16.77319139</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>36456.0</v>
+        <v>36032.0</v>
       </c>
       <c r="F5" s="7" t="n">
-        <v>42.8020079</v>
+        <v>46.00105462</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>2.53656463</v>
+        <v>2.74253441</v>
       </c>
       <c r="H5" s="7" t="n">
-        <v>236.0</v>
+        <v>244.0</v>
       </c>
       <c r="I5" s="7" t="n">
-        <v>6.61182203</v>
+        <v>6.79307377</v>
       </c>
       <c r="J5" s="7" t="n">
-        <v>0.25520963</v>
+        <v>0.24691608</v>
       </c>
       <c r="K5" s="7" t="n">
-        <v>161.0</v>
+        <v>180.0</v>
       </c>
       <c r="L5" s="7" t="n">
-        <v>9.69186335</v>
+        <v>9.20838889</v>
       </c>
       <c r="M5" s="7" t="n">
-        <v>14.0</v>
+        <v>20.0</v>
       </c>
       <c r="N5" s="7" t="n">
-        <v>111.45642857</v>
+        <v>82.8755</v>
       </c>
       <c r="O5" s="7" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="P5" s="7" t="n">
-        <v>1560.39</v>
+        <v>414.3775</v>
       </c>
       <c r="Q5" s="7" t="n">
-        <v>17.48</v>
+        <v>5090.86</v>
       </c>
       <c r="R5" s="7" t="n">
-        <v>0.01120233</v>
+        <v>3.07139022</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>1918.97</v>
+        <v>1680.14</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>95059.0</v>
+        <v>115943.0</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>20.18714693</v>
+        <v>14.49108614</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>47989.0</v>
+        <v>47279.0</v>
       </c>
       <c r="F6" s="7" t="n">
-        <v>39.98770552</v>
+        <v>35.53670763</v>
       </c>
       <c r="G6" s="7" t="n">
-        <v>1.98084978</v>
+        <v>2.45231498</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>278.0</v>
+        <v>316.0</v>
       </c>
       <c r="I6" s="7" t="n">
-        <v>6.90276978</v>
+        <v>5.31689873</v>
       </c>
       <c r="J6" s="7" t="n">
-        <v>0.29244995</v>
+        <v>0.27254772</v>
       </c>
       <c r="K6" s="7" t="n">
-        <v>215.0</v>
+        <v>199.0</v>
       </c>
       <c r="L6" s="7" t="n">
-        <v>8.92544186</v>
+        <v>8.44291457</v>
       </c>
       <c r="M6" s="7" t="n">
-        <v>22.0</v>
+        <v>13.0</v>
       </c>
       <c r="N6" s="7" t="n">
-        <v>87.22590909</v>
+        <v>129.24153846</v>
       </c>
       <c r="O6" s="7" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="P6" s="7" t="n">
-        <v>274.13857143</v>
+        <v>280.02333333</v>
       </c>
       <c r="Q6" s="7" t="n">
-        <v>6165.9</v>
+        <v>9050.3</v>
       </c>
       <c r="R6" s="7" t="n">
-        <v>3.21312996</v>
+        <v>5.38663445</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>1764.59</v>
+        <v>1526.13</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>113336.0</v>
+        <v>93257.0</v>
       </c>
       <c r="D7" s="7" t="n">
-        <v>15.56954542</v>
+        <v>16.36477691</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>55448.0</v>
+        <v>39210.0</v>
       </c>
       <c r="F7" s="7" t="n">
-        <v>31.82423171</v>
+        <v>38.92195868</v>
       </c>
       <c r="G7" s="7" t="n">
-        <v>2.04400519</v>
+        <v>2.37839837</v>
       </c>
       <c r="H7" s="7" t="n">
-        <v>447.0</v>
+        <v>241.0</v>
       </c>
       <c r="I7" s="7" t="n">
-        <v>3.94762864</v>
+        <v>6.33248963</v>
       </c>
       <c r="J7" s="7" t="n">
-        <v>0.39440248</v>
+        <v>0.25842564</v>
       </c>
       <c r="K7" s="7" t="n">
-        <v>311.0</v>
+        <v>165.0</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>5.67392283</v>
+        <v>9.24927273</v>
       </c>
       <c r="M7" s="7" t="n">
-        <v>15.0</v>
+        <v>3.0</v>
       </c>
       <c r="N7" s="7" t="n">
-        <v>117.63933333</v>
-      </c>
-      <c r="O7" s="7" t="s">
+        <v>508.71</v>
+      </c>
+      <c r="O7" s="7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="P7" s="7" t="n">
+        <v>381.5325</v>
+      </c>
+      <c r="Q7" s="7" t="n">
+        <v>3468.66</v>
+      </c>
+      <c r="R7" s="7" t="n">
+        <v>2.27284701</v>
+      </c>
+      <c r="S7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="T7" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -1006,55 +1018,55 @@
         <v>27</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>1729.47</v>
+        <v>1531.39</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>114695.0</v>
+        <v>94191.0</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>15.07886133</v>
+        <v>16.2583474</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>56275.0</v>
+        <v>43048.0</v>
       </c>
       <c r="F8" s="7" t="n">
-        <v>30.73247446</v>
+        <v>35.57401041</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>2.03811639</v>
+        <v>2.1880459</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>451.0</v>
+        <v>268.0</v>
       </c>
       <c r="I8" s="7" t="n">
-        <v>3.83474501</v>
+        <v>5.71414179</v>
       </c>
       <c r="J8" s="7" t="n">
-        <v>0.39321679</v>
+        <v>0.28452825</v>
       </c>
       <c r="K8" s="7" t="n">
-        <v>312.0</v>
+        <v>197.0</v>
       </c>
       <c r="L8" s="7" t="n">
-        <v>5.54317308</v>
+        <v>7.7735533</v>
       </c>
       <c r="M8" s="7" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="N8" s="7" t="n">
+        <v>47.8559375</v>
+      </c>
+      <c r="O8" s="7" t="n">
         <v>12.0</v>
       </c>
-      <c r="N8" s="7" t="n">
-        <v>144.1225</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>26</v>
+      <c r="P8" s="7" t="n">
+        <v>127.61583333</v>
+      </c>
+      <c r="Q8" s="7" t="n">
+        <v>5732.79</v>
+      </c>
+      <c r="R8" s="7" t="n">
+        <v>3.74352059</v>
       </c>
       <c r="S8" s="8" t="s">
         <v>27</v>
@@ -1068,55 +1080,55 @@
         <v>28</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>1675.4</v>
+        <v>1560.39</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>102285.0</v>
+        <v>92473.0</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>16.37972332</v>
+        <v>16.87400647</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>51781.0</v>
+        <v>36456.0</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>32.35549719</v>
+        <v>42.8020079</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>1.97533844</v>
+        <v>2.53656463</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>404.0</v>
+        <v>236.0</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>4.1470297</v>
+        <v>6.61182203</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>0.39497483</v>
+        <v>0.25520963</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>274.0</v>
+        <v>161.0</v>
       </c>
       <c r="L9" s="7" t="n">
-        <v>6.11459854</v>
+        <v>9.69186335</v>
       </c>
       <c r="M9" s="7" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="N9" s="7" t="n">
-        <v>128.87692308</v>
+        <v>111.45642857</v>
       </c>
       <c r="O9" s="7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="P9" s="7" t="n">
-        <v>837.7</v>
+        <v>1560.39</v>
       </c>
       <c r="Q9" s="7" t="n">
-        <v>6572.25</v>
+        <v>17.48</v>
       </c>
       <c r="R9" s="7" t="n">
-        <v>3.92279456</v>
+        <v>0.01120233</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>28</v>
@@ -1130,55 +1142,55 @@
         <v>29</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>1539.32</v>
+        <v>1918.97</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>91392.0</v>
+        <v>95059.0</v>
       </c>
       <c r="D10" s="7" t="n">
-        <v>16.84304972</v>
+        <v>20.18714693</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>44764.0</v>
+        <v>47989.0</v>
       </c>
       <c r="F10" s="7" t="n">
-        <v>34.3874542</v>
+        <v>39.98770552</v>
       </c>
       <c r="G10" s="7" t="n">
-        <v>2.0416406</v>
+        <v>1.98084978</v>
       </c>
       <c r="H10" s="7" t="n">
-        <v>319.0</v>
+        <v>278.0</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>4.82545455</v>
+        <v>6.90276978</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>0.34904587</v>
+        <v>0.29244995</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>237.0</v>
+        <v>215.0</v>
       </c>
       <c r="L10" s="7" t="n">
-        <v>6.4950211</v>
+        <v>8.92544186</v>
       </c>
       <c r="M10" s="7" t="n">
-        <v>11.0</v>
+        <v>22.0</v>
       </c>
       <c r="N10" s="7" t="n">
-        <v>139.93818182</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>26</v>
+        <v>87.22590909</v>
+      </c>
+      <c r="O10" s="7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="P10" s="7" t="n">
+        <v>274.13857143</v>
+      </c>
+      <c r="Q10" s="7" t="n">
+        <v>6165.9</v>
+      </c>
+      <c r="R10" s="7" t="n">
+        <v>3.21312996</v>
       </c>
       <c r="S10" s="8" t="s">
         <v>29</v>
@@ -1192,55 +1204,55 @@
         <v>30</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>1539.0</v>
+        <v>1764.59</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>96482.0</v>
+        <v>113336.0</v>
       </c>
       <c r="D11" s="7" t="n">
-        <v>15.95116187</v>
+        <v>15.56954542</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>45092.0</v>
+        <v>55448.0</v>
       </c>
       <c r="F11" s="7" t="n">
-        <v>34.13022266</v>
+        <v>31.82423171</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>2.13967001</v>
+        <v>2.04400519</v>
       </c>
       <c r="H11" s="7" t="n">
-        <v>325.0</v>
+        <v>447.0</v>
       </c>
       <c r="I11" s="7" t="n">
-        <v>4.73538462</v>
+        <v>3.94762864</v>
       </c>
       <c r="J11" s="7" t="n">
-        <v>0.3368504</v>
+        <v>0.39440248</v>
       </c>
       <c r="K11" s="7" t="n">
-        <v>236.0</v>
+        <v>311.0</v>
       </c>
       <c r="L11" s="7" t="n">
-        <v>6.52118644</v>
+        <v>5.67392283</v>
       </c>
       <c r="M11" s="7" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="N11" s="7" t="n">
-        <v>128.25</v>
-      </c>
-      <c r="O11" s="7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="P11" s="7" t="n">
-        <v>513.0</v>
-      </c>
-      <c r="Q11" s="7" t="n">
-        <v>5094.89</v>
-      </c>
-      <c r="R11" s="7" t="n">
-        <v>3.31051982</v>
+        <v>117.63933333</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>30</v>
@@ -1254,55 +1266,55 @@
         <v>31</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>1551.4</v>
+        <v>1729.47</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>82740.0</v>
+        <v>114695.0</v>
       </c>
       <c r="D12" s="7" t="n">
-        <v>18.75030215</v>
+        <v>15.07886133</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>38902.0</v>
+        <v>56275.0</v>
       </c>
       <c r="F12" s="7" t="n">
-        <v>39.8796977</v>
+        <v>30.73247446</v>
       </c>
       <c r="G12" s="7" t="n">
-        <v>2.12688294</v>
+        <v>2.03811639</v>
       </c>
       <c r="H12" s="7" t="n">
-        <v>294.0</v>
+        <v>451.0</v>
       </c>
       <c r="I12" s="7" t="n">
-        <v>5.27687075</v>
+        <v>3.83474501</v>
       </c>
       <c r="J12" s="7" t="n">
-        <v>0.35532995</v>
+        <v>0.39321679</v>
       </c>
       <c r="K12" s="7" t="n">
-        <v>214.0</v>
+        <v>312.0</v>
       </c>
       <c r="L12" s="7" t="n">
-        <v>7.24953271</v>
+        <v>5.54317308</v>
       </c>
       <c r="M12" s="7" t="n">
-        <v>19.0</v>
+        <v>12.0</v>
       </c>
       <c r="N12" s="7" t="n">
-        <v>81.65263158</v>
-      </c>
-      <c r="O12" s="7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="P12" s="7" t="n">
-        <v>517.13333333</v>
-      </c>
-      <c r="Q12" s="7" t="n">
-        <v>6065.01</v>
-      </c>
-      <c r="R12" s="7" t="n">
-        <v>3.90937863</v>
+        <v>144.1225</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="S12" s="8" t="s">
         <v>31</v>
@@ -1316,55 +1328,55 @@
         <v>32</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>1467.87</v>
+        <v>1675.4</v>
       </c>
       <c r="C13" s="6" t="n">
-        <v>71373.0</v>
+        <v>102285.0</v>
       </c>
       <c r="D13" s="7" t="n">
-        <v>20.56618049</v>
+        <v>16.37972332</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>36475.0</v>
+        <v>51781.0</v>
       </c>
       <c r="F13" s="7" t="n">
-        <v>40.24318026</v>
+        <v>32.35549719</v>
       </c>
       <c r="G13" s="7" t="n">
-        <v>1.95676491</v>
+        <v>1.97533844</v>
       </c>
       <c r="H13" s="7" t="n">
-        <v>246.0</v>
+        <v>404.0</v>
       </c>
       <c r="I13" s="7" t="n">
-        <v>5.96695122</v>
+        <v>4.1470297</v>
       </c>
       <c r="J13" s="7" t="n">
-        <v>0.34466815</v>
+        <v>0.39497483</v>
       </c>
       <c r="K13" s="7" t="n">
-        <v>195.0</v>
+        <v>274.0</v>
       </c>
       <c r="L13" s="7" t="n">
-        <v>7.52753846</v>
+        <v>6.11459854</v>
       </c>
       <c r="M13" s="7" t="n">
-        <v>17.0</v>
+        <v>13.0</v>
       </c>
       <c r="N13" s="7" t="n">
-        <v>86.34529412</v>
+        <v>128.87692308</v>
       </c>
       <c r="O13" s="7" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="P13" s="7" t="n">
-        <v>366.9675</v>
+        <v>837.7</v>
       </c>
       <c r="Q13" s="7" t="n">
-        <v>6023.34</v>
+        <v>6572.25</v>
       </c>
       <c r="R13" s="7" t="n">
-        <v>4.10345603</v>
+        <v>3.92279456</v>
       </c>
       <c r="S13" s="8" t="s">
         <v>32</v>
@@ -1378,55 +1390,55 @@
         <v>33</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>1285.98</v>
+        <v>1539.32</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>59799.0</v>
+        <v>91392.0</v>
       </c>
       <c r="D14" s="7" t="n">
-        <v>21.50504189</v>
+        <v>16.84304972</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>31208.0</v>
+        <v>44764.0</v>
       </c>
       <c r="F14" s="7" t="n">
-        <v>41.20674186</v>
+        <v>34.3874542</v>
       </c>
       <c r="G14" s="7" t="n">
-        <v>1.9161433</v>
+        <v>2.0416406</v>
       </c>
       <c r="H14" s="7" t="n">
-        <v>248.0</v>
+        <v>319.0</v>
       </c>
       <c r="I14" s="7" t="n">
-        <v>5.18540323</v>
+        <v>4.82545455</v>
       </c>
       <c r="J14" s="7" t="n">
-        <v>0.41472265</v>
+        <v>0.34904587</v>
       </c>
       <c r="K14" s="7" t="n">
-        <v>196.0</v>
+        <v>237.0</v>
       </c>
       <c r="L14" s="7" t="n">
-        <v>6.56112245</v>
+        <v>6.4950211</v>
       </c>
       <c r="M14" s="7" t="n">
-        <v>19.0</v>
+        <v>11.0</v>
       </c>
       <c r="N14" s="7" t="n">
-        <v>67.68315789</v>
-      </c>
-      <c r="O14" s="7" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="P14" s="7" t="n">
-        <v>257.196</v>
-      </c>
-      <c r="Q14" s="7" t="n">
-        <v>5438.57</v>
-      </c>
-      <c r="R14" s="7" t="n">
-        <v>4.22912487</v>
+        <v>139.93818182</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="S14" s="8" t="s">
         <v>33</v>
@@ -1440,55 +1452,55 @@
         <v>34</v>
       </c>
       <c r="B15" s="5" t="n">
-        <v>1166.86</v>
+        <v>1539.0</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>54762.0</v>
+        <v>96482.0</v>
       </c>
       <c r="D15" s="7" t="n">
-        <v>21.3078412</v>
+        <v>15.95116187</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>27770.0</v>
+        <v>45092.0</v>
       </c>
       <c r="F15" s="7" t="n">
-        <v>42.01872524</v>
+        <v>34.13022266</v>
       </c>
       <c r="G15" s="7" t="n">
-        <v>1.97198416</v>
+        <v>2.13967001</v>
       </c>
       <c r="H15" s="7" t="n">
-        <v>185.0</v>
+        <v>325.0</v>
       </c>
       <c r="I15" s="7" t="n">
-        <v>6.30735135</v>
+        <v>4.73538462</v>
       </c>
       <c r="J15" s="7" t="n">
-        <v>0.3378255</v>
+        <v>0.3368504</v>
       </c>
       <c r="K15" s="7" t="n">
-        <v>143.0</v>
+        <v>236.0</v>
       </c>
       <c r="L15" s="7" t="n">
-        <v>8.15986014</v>
+        <v>6.52118644</v>
       </c>
       <c r="M15" s="7" t="n">
-        <v>43.0</v>
+        <v>12.0</v>
       </c>
       <c r="N15" s="7" t="n">
-        <v>27.13627907</v>
+        <v>128.25</v>
       </c>
       <c r="O15" s="7" t="n">
-        <v>14.0</v>
+        <v>3.0</v>
       </c>
       <c r="P15" s="7" t="n">
-        <v>83.34714286</v>
+        <v>513.0</v>
       </c>
       <c r="Q15" s="7" t="n">
-        <v>10430.73</v>
+        <v>5094.89</v>
       </c>
       <c r="R15" s="7" t="n">
-        <v>8.93914437</v>
+        <v>3.31051982</v>
       </c>
       <c r="S15" s="8" t="s">
         <v>34</v>
@@ -1502,55 +1514,55 @@
         <v>35</v>
       </c>
       <c r="B16" s="5" t="n">
-        <v>1213.3</v>
+        <v>1551.4</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>51030.0</v>
+        <v>82740.0</v>
       </c>
       <c r="D16" s="7" t="n">
-        <v>23.77621007</v>
+        <v>18.75030215</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>25488.0</v>
+        <v>38902.0</v>
       </c>
       <c r="F16" s="7" t="n">
-        <v>47.60279347</v>
+        <v>39.8796977</v>
       </c>
       <c r="G16" s="7" t="n">
-        <v>2.00211864</v>
+        <v>2.12688294</v>
       </c>
       <c r="H16" s="7" t="n">
-        <v>224.0</v>
+        <v>294.0</v>
       </c>
       <c r="I16" s="7" t="n">
-        <v>5.41651786</v>
+        <v>5.27687075</v>
       </c>
       <c r="J16" s="7" t="n">
-        <v>0.43895748</v>
+        <v>0.35532995</v>
       </c>
       <c r="K16" s="7" t="n">
-        <v>181.0</v>
+        <v>214.0</v>
       </c>
       <c r="L16" s="7" t="n">
-        <v>6.70331492</v>
+        <v>7.24953271</v>
       </c>
       <c r="M16" s="7" t="n">
-        <v>16.0</v>
+        <v>19.0</v>
       </c>
       <c r="N16" s="7" t="n">
-        <v>75.83125</v>
+        <v>81.65263158</v>
       </c>
       <c r="O16" s="7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="P16" s="7" t="n">
-        <v>1213.3</v>
+        <v>517.13333333</v>
       </c>
       <c r="Q16" s="7" t="n">
-        <v>2783.21</v>
+        <v>6065.01</v>
       </c>
       <c r="R16" s="7" t="n">
-        <v>2.29391742</v>
+        <v>3.90937863</v>
       </c>
       <c r="S16" s="8" t="s">
         <v>35</v>
@@ -1564,55 +1576,55 @@
         <v>36</v>
       </c>
       <c r="B17" s="5" t="n">
-        <v>1160.45</v>
+        <v>1467.87</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>52438.0</v>
+        <v>71373.0</v>
       </c>
       <c r="D17" s="7" t="n">
-        <v>22.12994393</v>
+        <v>20.56618049</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>25276.0</v>
+        <v>36475.0</v>
       </c>
       <c r="F17" s="7" t="n">
-        <v>45.911141</v>
+        <v>40.24318026</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>2.07461624</v>
+        <v>1.95676491</v>
       </c>
       <c r="H17" s="7" t="n">
-        <v>229.0</v>
+        <v>246.0</v>
       </c>
       <c r="I17" s="7" t="n">
-        <v>5.06746725</v>
+        <v>5.96695122</v>
       </c>
       <c r="J17" s="7" t="n">
-        <v>0.43670621</v>
+        <v>0.34466815</v>
       </c>
       <c r="K17" s="7" t="n">
-        <v>190.0</v>
+        <v>195.0</v>
       </c>
       <c r="L17" s="7" t="n">
-        <v>6.10763158</v>
+        <v>7.52753846</v>
       </c>
       <c r="M17" s="7" t="n">
-        <v>13.0</v>
+        <v>17.0</v>
       </c>
       <c r="N17" s="7" t="n">
-        <v>89.26538462</v>
+        <v>86.34529412</v>
       </c>
       <c r="O17" s="7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="P17" s="7" t="n">
-        <v>580.225</v>
+        <v>366.9675</v>
       </c>
       <c r="Q17" s="7" t="n">
-        <v>4172.92</v>
+        <v>6023.34</v>
       </c>
       <c r="R17" s="7" t="n">
-        <v>3.59594985</v>
+        <v>4.10345603</v>
       </c>
       <c r="S17" s="8" t="s">
         <v>36</v>
@@ -1626,55 +1638,55 @@
         <v>37</v>
       </c>
       <c r="B18" s="5" t="n">
-        <v>1073.58</v>
+        <v>1285.98</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>48029.0</v>
+        <v>59799.0</v>
       </c>
       <c r="D18" s="7" t="n">
-        <v>22.35274522</v>
+        <v>21.50504189</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>23412.0</v>
+        <v>31208.0</v>
       </c>
       <c r="F18" s="7" t="n">
-        <v>45.8559713</v>
+        <v>41.20674186</v>
       </c>
       <c r="G18" s="7" t="n">
-        <v>2.05146933</v>
+        <v>1.9161433</v>
       </c>
       <c r="H18" s="7" t="n">
-        <v>240.0</v>
+        <v>248.0</v>
       </c>
       <c r="I18" s="7" t="n">
-        <v>4.47325</v>
+        <v>5.18540323</v>
       </c>
       <c r="J18" s="7" t="n">
-        <v>0.4996981</v>
+        <v>0.41472265</v>
       </c>
       <c r="K18" s="7" t="n">
-        <v>198.0</v>
+        <v>196.0</v>
       </c>
       <c r="L18" s="7" t="n">
-        <v>5.42212121</v>
+        <v>6.56112245</v>
       </c>
       <c r="M18" s="7" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="N18" s="7" t="n">
-        <v>59.64333333</v>
+        <v>67.68315789</v>
       </c>
       <c r="O18" s="7" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="P18" s="7" t="n">
-        <v>268.395</v>
+        <v>257.196</v>
       </c>
       <c r="Q18" s="7" t="n">
-        <v>8454.76</v>
+        <v>5438.57</v>
       </c>
       <c r="R18" s="7" t="n">
-        <v>7.87529574</v>
+        <v>4.22912487</v>
       </c>
       <c r="S18" s="8" t="s">
         <v>37</v>
@@ -1688,55 +1700,55 @@
         <v>38</v>
       </c>
       <c r="B19" s="5" t="n">
-        <v>1135.4</v>
+        <v>1166.86</v>
       </c>
       <c r="C19" s="6" t="n">
-        <v>51107.0</v>
+        <v>54762.0</v>
       </c>
       <c r="D19" s="7" t="n">
-        <v>22.21613478</v>
+        <v>21.3078412</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>23570.0</v>
+        <v>27770.0</v>
       </c>
       <c r="F19" s="7" t="n">
-        <v>48.17140433</v>
+        <v>42.01872524</v>
       </c>
       <c r="G19" s="7" t="n">
-        <v>2.16830717</v>
+        <v>1.97198416</v>
       </c>
       <c r="H19" s="7" t="n">
-        <v>202.0</v>
+        <v>185.0</v>
       </c>
       <c r="I19" s="7" t="n">
-        <v>5.62079208</v>
+        <v>6.30735135</v>
       </c>
       <c r="J19" s="7" t="n">
-        <v>0.39524918</v>
+        <v>0.3378255</v>
       </c>
       <c r="K19" s="7" t="n">
-        <v>173.0</v>
+        <v>143.0</v>
       </c>
       <c r="L19" s="7" t="n">
-        <v>6.56300578</v>
+        <v>8.15986014</v>
       </c>
       <c r="M19" s="7" t="n">
-        <v>10.0</v>
+        <v>43.0</v>
       </c>
       <c r="N19" s="7" t="n">
-        <v>113.54</v>
+        <v>27.13627907</v>
       </c>
       <c r="O19" s="7" t="n">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
       <c r="P19" s="7" t="n">
-        <v>1135.4</v>
+        <v>83.34714286</v>
       </c>
       <c r="Q19" s="7" t="n">
-        <v>2783.21</v>
+        <v>10430.73</v>
       </c>
       <c r="R19" s="7" t="n">
-        <v>2.45130351</v>
+        <v>8.93914437</v>
       </c>
       <c r="S19" s="8" t="s">
         <v>38</v>
@@ -1750,55 +1762,55 @@
         <v>39</v>
       </c>
       <c r="B20" s="5" t="n">
-        <v>1031.99</v>
+        <v>1213.3</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>47146.0</v>
+        <v>51030.0</v>
       </c>
       <c r="D20" s="7" t="n">
-        <v>21.88923769</v>
+        <v>23.77621007</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>21231.0</v>
+        <v>25488.0</v>
       </c>
       <c r="F20" s="7" t="n">
-        <v>48.60769629</v>
+        <v>47.60279347</v>
       </c>
       <c r="G20" s="7" t="n">
-        <v>2.22062079</v>
+        <v>2.00211864</v>
       </c>
       <c r="H20" s="7" t="n">
-        <v>205.0</v>
+        <v>224.0</v>
       </c>
       <c r="I20" s="7" t="n">
-        <v>5.03409756</v>
+        <v>5.41651786</v>
       </c>
       <c r="J20" s="7" t="n">
-        <v>0.4348195</v>
+        <v>0.43895748</v>
       </c>
       <c r="K20" s="7" t="n">
-        <v>161.0</v>
+        <v>181.0</v>
       </c>
       <c r="L20" s="7" t="n">
-        <v>6.40987578</v>
+        <v>6.70331492</v>
       </c>
       <c r="M20" s="7" t="n">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="N20" s="7" t="n">
-        <v>60.70529412</v>
+        <v>75.83125</v>
       </c>
       <c r="O20" s="7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="P20" s="7" t="n">
-        <v>515.995</v>
+        <v>1213.3</v>
       </c>
       <c r="Q20" s="7" t="n">
-        <v>4637.42</v>
+        <v>2783.21</v>
       </c>
       <c r="R20" s="7" t="n">
-        <v>4.49366757</v>
+        <v>2.29391742</v>
       </c>
       <c r="S20" s="8" t="s">
         <v>39</v>
@@ -1812,55 +1824,55 @@
         <v>40</v>
       </c>
       <c r="B21" s="5" t="n">
-        <v>965.49</v>
+        <v>1160.45</v>
       </c>
       <c r="C21" s="6" t="n">
-        <v>44465.0</v>
+        <v>52438.0</v>
       </c>
       <c r="D21" s="7" t="n">
-        <v>21.71348251</v>
+        <v>22.12994393</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>19909.0</v>
+        <v>25276.0</v>
       </c>
       <c r="F21" s="7" t="n">
-        <v>48.49515295</v>
+        <v>45.911141</v>
       </c>
       <c r="G21" s="7" t="n">
-        <v>2.23341202</v>
+        <v>2.07461624</v>
       </c>
       <c r="H21" s="7" t="n">
-        <v>182.0</v>
+        <v>229.0</v>
       </c>
       <c r="I21" s="7" t="n">
-        <v>5.30489011</v>
+        <v>5.06746725</v>
       </c>
       <c r="J21" s="7" t="n">
-        <v>0.40931069</v>
+        <v>0.43670621</v>
       </c>
       <c r="K21" s="7" t="n">
-        <v>132.0</v>
+        <v>190.0</v>
       </c>
       <c r="L21" s="7" t="n">
-        <v>7.31431818</v>
+        <v>6.10763158</v>
       </c>
       <c r="M21" s="7" t="n">
-        <v>16.0</v>
+        <v>13.0</v>
       </c>
       <c r="N21" s="7" t="n">
-        <v>60.343125</v>
+        <v>89.26538462</v>
       </c>
       <c r="O21" s="7" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="P21" s="7" t="n">
-        <v>193.098</v>
+        <v>580.225</v>
       </c>
       <c r="Q21" s="7" t="n">
-        <v>12277.19</v>
+        <v>4172.92</v>
       </c>
       <c r="R21" s="7" t="n">
-        <v>12.71601984</v>
+        <v>3.59594985</v>
       </c>
       <c r="S21" s="8" t="s">
         <v>40</v>
@@ -1874,55 +1886,55 @@
         <v>41</v>
       </c>
       <c r="B22" s="5" t="n">
-        <v>989.99</v>
+        <v>1073.58</v>
       </c>
       <c r="C22" s="6" t="n">
-        <v>54770.0</v>
+        <v>48029.0</v>
       </c>
       <c r="D22" s="7" t="n">
-        <v>18.07540624</v>
+        <v>22.35274522</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>24689.0</v>
+        <v>23412.0</v>
       </c>
       <c r="F22" s="7" t="n">
-        <v>40.0984244</v>
+        <v>45.8559713</v>
       </c>
       <c r="G22" s="7" t="n">
-        <v>2.21839686</v>
+        <v>2.05146933</v>
       </c>
       <c r="H22" s="7" t="n">
-        <v>171.0</v>
+        <v>240.0</v>
       </c>
       <c r="I22" s="7" t="n">
-        <v>5.7894152</v>
+        <v>4.47325</v>
       </c>
       <c r="J22" s="7" t="n">
-        <v>0.31221472</v>
+        <v>0.4996981</v>
       </c>
       <c r="K22" s="7" t="n">
-        <v>143.0</v>
+        <v>198.0</v>
       </c>
       <c r="L22" s="7" t="n">
-        <v>6.92300699</v>
+        <v>5.42212121</v>
       </c>
       <c r="M22" s="7" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="N22" s="7" t="n">
+        <v>59.64333333</v>
+      </c>
+      <c r="O22" s="7" t="n">
         <v>4.0</v>
       </c>
-      <c r="N22" s="7" t="n">
-        <v>247.4975</v>
-      </c>
-      <c r="O22" s="7" t="n">
-        <v>2.0</v>
-      </c>
       <c r="P22" s="7" t="n">
-        <v>494.995</v>
+        <v>268.395</v>
       </c>
       <c r="Q22" s="7" t="n">
-        <v>2779.42</v>
+        <v>8454.76</v>
       </c>
       <c r="R22" s="7" t="n">
-        <v>2.80752331</v>
+        <v>7.87529574</v>
       </c>
       <c r="S22" s="8" t="s">
         <v>41</v>
@@ -1936,55 +1948,55 @@
         <v>42</v>
       </c>
       <c r="B23" s="5" t="n">
-        <v>985.8</v>
+        <v>1135.4</v>
       </c>
       <c r="C23" s="6" t="n">
-        <v>48715.0</v>
+        <v>51107.0</v>
       </c>
       <c r="D23" s="7" t="n">
-        <v>20.23606692</v>
+        <v>22.21613478</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>22229.0</v>
+        <v>23570.0</v>
       </c>
       <c r="F23" s="7" t="n">
-        <v>44.34747402</v>
+        <v>48.17140433</v>
       </c>
       <c r="G23" s="7" t="n">
-        <v>2.19150659</v>
+        <v>2.16830717</v>
       </c>
       <c r="H23" s="7" t="n">
-        <v>190.0</v>
+        <v>202.0</v>
       </c>
       <c r="I23" s="7" t="n">
-        <v>5.18842105</v>
+        <v>5.62079208</v>
       </c>
       <c r="J23" s="7" t="n">
-        <v>0.39002361</v>
+        <v>0.39524918</v>
       </c>
       <c r="K23" s="7" t="n">
-        <v>140.0</v>
+        <v>173.0</v>
       </c>
       <c r="L23" s="7" t="n">
-        <v>7.04142857</v>
+        <v>6.56300578</v>
       </c>
       <c r="M23" s="7" t="n">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
       <c r="N23" s="7" t="n">
-        <v>75.83076923</v>
+        <v>113.54</v>
       </c>
       <c r="O23" s="7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="P23" s="7" t="n">
-        <v>492.9</v>
+        <v>1135.4</v>
       </c>
       <c r="Q23" s="7" t="n">
-        <v>4631.86</v>
+        <v>2783.21</v>
       </c>
       <c r="R23" s="7" t="n">
-        <v>4.69857983</v>
+        <v>2.45130351</v>
       </c>
       <c r="S23" s="8" t="s">
         <v>42</v>
@@ -1998,55 +2010,55 @@
         <v>43</v>
       </c>
       <c r="B24" s="5" t="n">
-        <v>916.13</v>
+        <v>1031.99</v>
       </c>
       <c r="C24" s="6" t="n">
-        <v>41225.0</v>
+        <v>47146.0</v>
       </c>
       <c r="D24" s="7" t="n">
-        <v>22.22268041</v>
+        <v>21.88923769</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>18895.0</v>
+        <v>21231.0</v>
       </c>
       <c r="F24" s="7" t="n">
-        <v>48.48531358</v>
+        <v>48.60769629</v>
       </c>
       <c r="G24" s="7" t="n">
-        <v>2.18179413</v>
+        <v>2.22062079</v>
       </c>
       <c r="H24" s="7" t="n">
-        <v>174.0</v>
+        <v>205.0</v>
       </c>
       <c r="I24" s="7" t="n">
-        <v>5.26511494</v>
+        <v>5.03409756</v>
       </c>
       <c r="J24" s="7" t="n">
-        <v>0.42207398</v>
+        <v>0.4348195</v>
       </c>
       <c r="K24" s="7" t="n">
-        <v>139.0</v>
+        <v>161.0</v>
       </c>
       <c r="L24" s="7" t="n">
-        <v>6.59086331</v>
+        <v>6.40987578</v>
       </c>
       <c r="M24" s="7" t="n">
-        <v>5.0</v>
+        <v>17.0</v>
       </c>
       <c r="N24" s="7" t="n">
-        <v>183.226</v>
-      </c>
-      <c r="O24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>26</v>
+        <v>60.70529412</v>
+      </c>
+      <c r="O24" s="7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P24" s="7" t="n">
+        <v>515.995</v>
+      </c>
+      <c r="Q24" s="7" t="n">
+        <v>4637.42</v>
+      </c>
+      <c r="R24" s="7" t="n">
+        <v>4.49366757</v>
       </c>
       <c r="S24" s="8" t="s">
         <v>43</v>
@@ -2060,55 +2072,55 @@
         <v>44</v>
       </c>
       <c r="B25" s="5" t="n">
-        <v>911.72</v>
+        <v>965.49</v>
       </c>
       <c r="C25" s="6" t="n">
-        <v>37615.0</v>
+        <v>44465.0</v>
       </c>
       <c r="D25" s="7" t="n">
-        <v>24.23820284</v>
+        <v>21.71348251</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>17072.0</v>
+        <v>19909.0</v>
       </c>
       <c r="F25" s="7" t="n">
-        <v>53.40440487</v>
+        <v>48.49515295</v>
       </c>
       <c r="G25" s="7" t="n">
-        <v>2.20331537</v>
+        <v>2.23341202</v>
       </c>
       <c r="H25" s="7" t="n">
-        <v>157.0</v>
+        <v>182.0</v>
       </c>
       <c r="I25" s="7" t="n">
-        <v>5.80713376</v>
+        <v>5.30489011</v>
       </c>
       <c r="J25" s="7" t="n">
-        <v>0.41738668</v>
+        <v>0.40931069</v>
       </c>
       <c r="K25" s="7" t="n">
-        <v>123.0</v>
+        <v>132.0</v>
       </c>
       <c r="L25" s="7" t="n">
-        <v>7.41235772</v>
+        <v>7.31431818</v>
       </c>
       <c r="M25" s="7" t="n">
-        <v>10.0</v>
+        <v>16.0</v>
       </c>
       <c r="N25" s="7" t="n">
-        <v>91.172</v>
-      </c>
-      <c r="O25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R25" s="7" t="s">
-        <v>26</v>
+        <v>60.343125</v>
+      </c>
+      <c r="O25" s="7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="P25" s="7" t="n">
+        <v>193.098</v>
+      </c>
+      <c r="Q25" s="7" t="n">
+        <v>12277.19</v>
+      </c>
+      <c r="R25" s="7" t="n">
+        <v>12.71601984</v>
       </c>
       <c r="S25" s="8" t="s">
         <v>44</v>
@@ -2122,55 +2134,55 @@
         <v>45</v>
       </c>
       <c r="B26" s="5" t="n">
-        <v>838.34</v>
+        <v>989.99</v>
       </c>
       <c r="C26" s="6" t="n">
-        <v>35648.0</v>
+        <v>54770.0</v>
       </c>
       <c r="D26" s="7" t="n">
-        <v>23.51716786</v>
+        <v>18.07540624</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>15767.0</v>
+        <v>24689.0</v>
       </c>
       <c r="F26" s="7" t="n">
-        <v>53.17054608</v>
+        <v>40.0984244</v>
       </c>
       <c r="G26" s="7" t="n">
-        <v>2.26092472</v>
+        <v>2.21839686</v>
       </c>
       <c r="H26" s="7" t="n">
-        <v>167.0</v>
+        <v>171.0</v>
       </c>
       <c r="I26" s="7" t="n">
-        <v>5.02</v>
+        <v>5.7894152</v>
       </c>
       <c r="J26" s="7" t="n">
-        <v>0.46846948</v>
+        <v>0.31221472</v>
       </c>
       <c r="K26" s="7" t="n">
-        <v>117.0</v>
+        <v>143.0</v>
       </c>
       <c r="L26" s="7" t="n">
-        <v>7.16529915</v>
+        <v>6.92300699</v>
       </c>
       <c r="M26" s="7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="N26" s="7" t="n">
+        <v>247.4975</v>
+      </c>
+      <c r="O26" s="7" t="n">
         <v>2.0</v>
       </c>
-      <c r="N26" s="7" t="n">
-        <v>419.17</v>
-      </c>
-      <c r="O26" s="7" t="n">
-        <v>1.0</v>
-      </c>
       <c r="P26" s="7" t="n">
-        <v>838.34</v>
+        <v>494.995</v>
       </c>
       <c r="Q26" s="7" t="n">
-        <v>925.21</v>
+        <v>2779.42</v>
       </c>
       <c r="R26" s="7" t="n">
-        <v>1.10362144</v>
+        <v>2.80752331</v>
       </c>
       <c r="S26" s="8" t="s">
         <v>45</v>
@@ -2184,55 +2196,55 @@
         <v>46</v>
       </c>
       <c r="B27" s="5" t="n">
-        <v>467.36</v>
+        <v>985.8</v>
       </c>
       <c r="C27" s="6" t="n">
-        <v>24162.0</v>
+        <v>48715.0</v>
       </c>
       <c r="D27" s="7" t="n">
-        <v>19.34276964</v>
+        <v>20.23606692</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>11638.0</v>
+        <v>22229.0</v>
       </c>
       <c r="F27" s="7" t="n">
-        <v>40.15810277</v>
+        <v>44.34747402</v>
       </c>
       <c r="G27" s="7" t="n">
-        <v>2.07612992</v>
+        <v>2.19150659</v>
       </c>
       <c r="H27" s="7" t="n">
-        <v>103.0</v>
+        <v>190.0</v>
       </c>
       <c r="I27" s="7" t="n">
-        <v>4.53747573</v>
+        <v>5.18842105</v>
       </c>
       <c r="J27" s="7" t="n">
-        <v>0.42628921</v>
+        <v>0.39002361</v>
       </c>
       <c r="K27" s="7" t="n">
-        <v>85.0</v>
+        <v>140.0</v>
       </c>
       <c r="L27" s="7" t="n">
-        <v>5.49835294</v>
+        <v>7.04142857</v>
       </c>
       <c r="M27" s="7" t="n">
-        <v>9.0</v>
+        <v>13.0</v>
       </c>
       <c r="N27" s="7" t="n">
-        <v>51.92888889</v>
+        <v>75.83076923</v>
       </c>
       <c r="O27" s="7" t="n">
         <v>2.0</v>
       </c>
       <c r="P27" s="7" t="n">
-        <v>233.68</v>
+        <v>492.9</v>
       </c>
       <c r="Q27" s="7" t="n">
-        <v>3708.42</v>
+        <v>4631.86</v>
       </c>
       <c r="R27" s="7" t="n">
-        <v>7.9348254</v>
+        <v>4.69857983</v>
       </c>
       <c r="S27" s="8" t="s">
         <v>46</v>
@@ -2246,55 +2258,55 @@
         <v>47</v>
       </c>
       <c r="B28" s="5" t="n">
-        <v>467.28</v>
+        <v>916.13</v>
       </c>
       <c r="C28" s="6" t="n">
-        <v>22806.0</v>
+        <v>41225.0</v>
       </c>
       <c r="D28" s="7" t="n">
-        <v>20.48934491</v>
+        <v>22.22268041</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>10028.0</v>
+        <v>18895.0</v>
       </c>
       <c r="F28" s="7" t="n">
-        <v>46.59752692</v>
+        <v>48.48531358</v>
       </c>
       <c r="G28" s="7" t="n">
-        <v>2.27423215</v>
+        <v>2.18179413</v>
       </c>
       <c r="H28" s="7" t="n">
-        <v>94.0</v>
+        <v>174.0</v>
       </c>
       <c r="I28" s="7" t="n">
-        <v>4.97106383</v>
+        <v>5.26511494</v>
       </c>
       <c r="J28" s="7" t="n">
-        <v>0.41217224</v>
+        <v>0.42207398</v>
       </c>
       <c r="K28" s="7" t="n">
-        <v>75.0</v>
+        <v>139.0</v>
       </c>
       <c r="L28" s="7" t="n">
-        <v>6.2304</v>
+        <v>6.59086331</v>
       </c>
       <c r="M28" s="7" t="n">
         <v>5.0</v>
       </c>
       <c r="N28" s="7" t="n">
-        <v>93.456</v>
+        <v>183.226</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Q28" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="R28" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S28" s="8" t="s">
         <v>47</v>
@@ -2308,55 +2320,55 @@
         <v>48</v>
       </c>
       <c r="B29" s="5" t="n">
-        <v>497.17</v>
+        <v>911.72</v>
       </c>
       <c r="C29" s="6" t="n">
-        <v>32963.0</v>
+        <v>37615.0</v>
       </c>
       <c r="D29" s="7" t="n">
-        <v>15.08266845</v>
+        <v>24.23820284</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>15164.0</v>
+        <v>17072.0</v>
       </c>
       <c r="F29" s="7" t="n">
-        <v>32.78620417</v>
+        <v>53.40440487</v>
       </c>
       <c r="G29" s="7" t="n">
-        <v>2.17376682</v>
+        <v>2.20331537</v>
       </c>
       <c r="H29" s="7" t="n">
-        <v>101.0</v>
+        <v>157.0</v>
       </c>
       <c r="I29" s="7" t="n">
-        <v>4.92247525</v>
+        <v>5.80713376</v>
       </c>
       <c r="J29" s="7" t="n">
-        <v>0.30640415</v>
+        <v>0.41738668</v>
       </c>
       <c r="K29" s="7" t="n">
-        <v>79.0</v>
+        <v>123.0</v>
       </c>
       <c r="L29" s="7" t="n">
-        <v>6.29329114</v>
+        <v>7.41235772</v>
       </c>
       <c r="M29" s="7" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="N29" s="7" t="n">
-        <v>82.86166667</v>
-      </c>
-      <c r="O29" s="7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="P29" s="7" t="n">
-        <v>165.72333333</v>
-      </c>
-      <c r="Q29" s="7" t="n">
-        <v>5559.85</v>
-      </c>
-      <c r="R29" s="7" t="n">
-        <v>11.18299576</v>
+        <v>91.172</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="S29" s="8" t="s">
         <v>48</v>
@@ -2370,55 +2382,55 @@
         <v>49</v>
       </c>
       <c r="B30" s="5" t="n">
-        <v>469.99</v>
+        <v>838.34</v>
       </c>
       <c r="C30" s="6" t="n">
-        <v>33990.0</v>
+        <v>35648.0</v>
       </c>
       <c r="D30" s="7" t="n">
-        <v>13.82730215</v>
+        <v>23.51716786</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>16837.0</v>
+        <v>15767.0</v>
       </c>
       <c r="F30" s="7" t="n">
-        <v>27.91411772</v>
+        <v>53.17054608</v>
       </c>
       <c r="G30" s="7" t="n">
-        <v>2.01876819</v>
+        <v>2.26092472</v>
       </c>
       <c r="H30" s="7" t="n">
-        <v>100.0</v>
+        <v>167.0</v>
       </c>
       <c r="I30" s="7" t="n">
-        <v>4.6999</v>
+        <v>5.02</v>
       </c>
       <c r="J30" s="7" t="n">
-        <v>0.29420418</v>
+        <v>0.46846948</v>
       </c>
       <c r="K30" s="7" t="n">
-        <v>90.0</v>
+        <v>117.0</v>
       </c>
       <c r="L30" s="7" t="n">
-        <v>5.22211111</v>
+        <v>7.16529915</v>
       </c>
       <c r="M30" s="7" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="N30" s="7" t="n">
-        <v>93.998</v>
+        <v>419.17</v>
       </c>
       <c r="O30" s="7" t="n">
         <v>1.0</v>
       </c>
       <c r="P30" s="7" t="n">
-        <v>469.99</v>
+        <v>838.34</v>
       </c>
       <c r="Q30" s="7" t="n">
         <v>925.21</v>
       </c>
       <c r="R30" s="7" t="n">
-        <v>1.9685738</v>
+        <v>1.10362144</v>
       </c>
       <c r="S30" s="8" t="s">
         <v>49</v>
@@ -2432,55 +2444,55 @@
         <v>50</v>
       </c>
       <c r="B31" s="5" t="n">
-        <v>442.22</v>
+        <v>467.36</v>
       </c>
       <c r="C31" s="6" t="n">
-        <v>33316.0</v>
+        <v>24162.0</v>
       </c>
       <c r="D31" s="7" t="n">
-        <v>13.27350222</v>
+        <v>19.34276964</v>
       </c>
       <c r="E31" s="6" t="n">
-        <v>16542.0</v>
+        <v>11638.0</v>
       </c>
       <c r="F31" s="7" t="n">
-        <v>26.73316407</v>
+        <v>40.15810277</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>2.01402491</v>
+        <v>2.07612992</v>
       </c>
       <c r="H31" s="7" t="n">
-        <v>82.0</v>
+        <v>103.0</v>
       </c>
       <c r="I31" s="7" t="n">
-        <v>5.39292683</v>
+        <v>4.53747573</v>
       </c>
       <c r="J31" s="7" t="n">
-        <v>0.24612799</v>
+        <v>0.42628921</v>
       </c>
       <c r="K31" s="7" t="n">
-        <v>76.0</v>
+        <v>85.0</v>
       </c>
       <c r="L31" s="7" t="n">
-        <v>5.81868421</v>
+        <v>5.49835294</v>
       </c>
       <c r="M31" s="7" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="N31" s="7" t="n">
+        <v>51.92888889</v>
+      </c>
+      <c r="O31" s="7" t="n">
         <v>2.0</v>
       </c>
-      <c r="N31" s="7" t="n">
-        <v>221.11</v>
-      </c>
-      <c r="O31" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P31" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q31" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R31" s="7" t="s">
-        <v>26</v>
+      <c r="P31" s="7" t="n">
+        <v>233.68</v>
+      </c>
+      <c r="Q31" s="7" t="n">
+        <v>3708.42</v>
+      </c>
+      <c r="R31" s="7" t="n">
+        <v>7.9348254</v>
       </c>
       <c r="S31" s="8" t="s">
         <v>50</v>
@@ -2494,55 +2506,55 @@
         <v>51</v>
       </c>
       <c r="B32" s="5" t="n">
-        <v>415.57</v>
+        <v>467.28</v>
       </c>
       <c r="C32" s="6" t="n">
-        <v>27930.0</v>
+        <v>22806.0</v>
       </c>
       <c r="D32" s="7" t="n">
-        <v>14.87898317</v>
+        <v>20.48934491</v>
       </c>
       <c r="E32" s="6" t="n">
-        <v>13818.0</v>
+        <v>10028.0</v>
       </c>
       <c r="F32" s="7" t="n">
-        <v>30.07454045</v>
+        <v>46.59752692</v>
       </c>
       <c r="G32" s="7" t="n">
-        <v>2.0212766</v>
+        <v>2.27423215</v>
       </c>
       <c r="H32" s="7" t="n">
-        <v>89.0</v>
+        <v>94.0</v>
       </c>
       <c r="I32" s="7" t="n">
-        <v>4.66932584</v>
+        <v>4.97106383</v>
       </c>
       <c r="J32" s="7" t="n">
-        <v>0.31865378</v>
+        <v>0.41217224</v>
       </c>
       <c r="K32" s="7" t="n">
-        <v>76.0</v>
+        <v>75.0</v>
       </c>
       <c r="L32" s="7" t="n">
-        <v>5.46802632</v>
+        <v>6.2304</v>
       </c>
       <c r="M32" s="7" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="N32" s="7" t="n">
-        <v>46.17444444</v>
+        <v>93.456</v>
       </c>
       <c r="O32" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Q32" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="R32" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S32" s="8" t="s">
         <v>51</v>
@@ -2556,55 +2568,55 @@
         <v>52</v>
       </c>
       <c r="B33" s="5" t="n">
-        <v>428.3</v>
+        <v>497.17</v>
       </c>
       <c r="C33" s="6" t="n">
-        <v>23286.0</v>
+        <v>32963.0</v>
       </c>
       <c r="D33" s="7" t="n">
-        <v>18.39302585</v>
+        <v>15.08266845</v>
       </c>
       <c r="E33" s="6" t="n">
-        <v>11410.0</v>
+        <v>15164.0</v>
       </c>
       <c r="F33" s="7" t="n">
-        <v>37.53724803</v>
+        <v>32.78620417</v>
       </c>
       <c r="G33" s="7" t="n">
-        <v>2.04084137</v>
+        <v>2.17376682</v>
       </c>
       <c r="H33" s="7" t="n">
-        <v>98.0</v>
+        <v>101.0</v>
       </c>
       <c r="I33" s="7" t="n">
-        <v>4.37040816</v>
+        <v>4.92247525</v>
       </c>
       <c r="J33" s="7" t="n">
-        <v>0.42085373</v>
+        <v>0.30640415</v>
       </c>
       <c r="K33" s="7" t="n">
-        <v>85.0</v>
+        <v>79.0</v>
       </c>
       <c r="L33" s="7" t="n">
-        <v>5.03882353</v>
+        <v>6.29329114</v>
       </c>
       <c r="M33" s="7" t="n">
-        <v>11.0</v>
+        <v>6.0</v>
       </c>
       <c r="N33" s="7" t="n">
-        <v>38.93636364</v>
+        <v>82.86166667</v>
       </c>
       <c r="O33" s="7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="P33" s="7" t="n">
-        <v>428.3</v>
+        <v>165.72333333</v>
       </c>
       <c r="Q33" s="7" t="n">
-        <v>1970.51</v>
+        <v>5559.85</v>
       </c>
       <c r="R33" s="7" t="n">
-        <v>4.60077049</v>
+        <v>11.18299576</v>
       </c>
       <c r="S33" s="8" t="s">
         <v>52</v>
@@ -2618,55 +2630,55 @@
         <v>53</v>
       </c>
       <c r="B34" s="5" t="n">
-        <v>422.78</v>
+        <v>469.99</v>
       </c>
       <c r="C34" s="6" t="n">
-        <v>21954.0</v>
+        <v>33990.0</v>
       </c>
       <c r="D34" s="7" t="n">
-        <v>19.25753849</v>
+        <v>13.82730215</v>
       </c>
       <c r="E34" s="6" t="n">
-        <v>11094.0</v>
+        <v>16837.0</v>
       </c>
       <c r="F34" s="7" t="n">
-        <v>38.10888769</v>
+        <v>27.91411772</v>
       </c>
       <c r="G34" s="7" t="n">
-        <v>1.97890752</v>
+        <v>2.01876819</v>
       </c>
       <c r="H34" s="7" t="n">
-        <v>75.0</v>
+        <v>100.0</v>
       </c>
       <c r="I34" s="7" t="n">
-        <v>5.63706667</v>
+        <v>4.6999</v>
       </c>
       <c r="J34" s="7" t="n">
-        <v>0.34162339</v>
+        <v>0.29420418</v>
       </c>
       <c r="K34" s="7" t="n">
-        <v>71.0</v>
+        <v>90.0</v>
       </c>
       <c r="L34" s="7" t="n">
-        <v>5.95464789</v>
+        <v>5.22211111</v>
       </c>
       <c r="M34" s="7" t="n">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="N34" s="7" t="n">
-        <v>42.278</v>
-      </c>
-      <c r="O34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R34" s="7" t="s">
-        <v>26</v>
+        <v>93.998</v>
+      </c>
+      <c r="O34" s="7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P34" s="7" t="n">
+        <v>469.99</v>
+      </c>
+      <c r="Q34" s="7" t="n">
+        <v>925.21</v>
+      </c>
+      <c r="R34" s="7" t="n">
+        <v>1.9685738</v>
       </c>
       <c r="S34" s="8" t="s">
         <v>53</v>
@@ -2680,55 +2692,55 @@
         <v>54</v>
       </c>
       <c r="B35" s="5" t="n">
-        <v>499.52</v>
+        <v>442.22</v>
       </c>
       <c r="C35" s="6" t="n">
-        <v>22339.0</v>
+        <v>33316.0</v>
       </c>
       <c r="D35" s="7" t="n">
-        <v>22.3608935</v>
+        <v>13.27350222</v>
       </c>
       <c r="E35" s="6" t="n">
-        <v>11535.0</v>
+        <v>16542.0</v>
       </c>
       <c r="F35" s="7" t="n">
-        <v>43.30472475</v>
+        <v>26.73316407</v>
       </c>
       <c r="G35" s="7" t="n">
-        <v>1.93662765</v>
+        <v>2.01402491</v>
       </c>
       <c r="H35" s="7" t="n">
-        <v>110.0</v>
+        <v>82.0</v>
       </c>
       <c r="I35" s="7" t="n">
-        <v>4.54109091</v>
+        <v>5.39292683</v>
       </c>
       <c r="J35" s="7" t="n">
-        <v>0.49241237</v>
+        <v>0.24612799</v>
       </c>
       <c r="K35" s="7" t="n">
-        <v>92.0</v>
+        <v>76.0</v>
       </c>
       <c r="L35" s="7" t="n">
-        <v>5.42956522</v>
+        <v>5.81868421</v>
       </c>
       <c r="M35" s="7" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="N35" s="7" t="n">
-        <v>62.44</v>
+        <v>221.11</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="R35" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S35" s="8" t="s">
         <v>54</v>
@@ -2742,55 +2754,55 @@
         <v>55</v>
       </c>
       <c r="B36" s="5" t="n">
-        <v>517.29</v>
+        <v>415.57</v>
       </c>
       <c r="C36" s="6" t="n">
-        <v>20548.0</v>
+        <v>27930.0</v>
       </c>
       <c r="D36" s="7" t="n">
-        <v>25.17471287</v>
+        <v>14.87898317</v>
       </c>
       <c r="E36" s="6" t="n">
-        <v>9854.0</v>
+        <v>13818.0</v>
       </c>
       <c r="F36" s="7" t="n">
-        <v>52.49543333</v>
+        <v>30.07454045</v>
       </c>
       <c r="G36" s="7" t="n">
-        <v>2.08524457</v>
+        <v>2.0212766</v>
       </c>
       <c r="H36" s="7" t="n">
-        <v>133.0</v>
+        <v>89.0</v>
       </c>
       <c r="I36" s="7" t="n">
-        <v>3.8893985</v>
+        <v>4.66932584</v>
       </c>
       <c r="J36" s="7" t="n">
-        <v>0.64726494</v>
+        <v>0.31865378</v>
       </c>
       <c r="K36" s="7" t="n">
-        <v>109.0</v>
+        <v>76.0</v>
       </c>
       <c r="L36" s="7" t="n">
-        <v>4.74577982</v>
+        <v>5.46802632</v>
       </c>
       <c r="M36" s="7" t="n">
-        <v>13.0</v>
+        <v>9.0</v>
       </c>
       <c r="N36" s="7" t="n">
-        <v>39.79153846</v>
-      </c>
-      <c r="O36" s="7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="P36" s="7" t="n">
-        <v>172.43</v>
-      </c>
-      <c r="Q36" s="7" t="n">
-        <v>3008.3</v>
-      </c>
-      <c r="R36" s="7" t="n">
-        <v>5.81550001</v>
+        <v>46.17444444</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R36" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="S36" s="8" t="s">
         <v>55</v>
@@ -2804,55 +2816,55 @@
         <v>56</v>
       </c>
       <c r="B37" s="5" t="n">
-        <v>523.08</v>
+        <v>428.3</v>
       </c>
       <c r="C37" s="6" t="n">
-        <v>17981.0</v>
+        <v>23286.0</v>
       </c>
       <c r="D37" s="7" t="n">
-        <v>29.09070686</v>
+        <v>18.39302585</v>
       </c>
       <c r="E37" s="6" t="n">
-        <v>9592.0</v>
+        <v>11410.0</v>
       </c>
       <c r="F37" s="7" t="n">
-        <v>54.53294412</v>
+        <v>37.53724803</v>
       </c>
       <c r="G37" s="7" t="n">
-        <v>1.87458299</v>
+        <v>2.04084137</v>
       </c>
       <c r="H37" s="7" t="n">
-        <v>92.0</v>
+        <v>98.0</v>
       </c>
       <c r="I37" s="7" t="n">
-        <v>5.68565217</v>
+        <v>4.37040816</v>
       </c>
       <c r="J37" s="7" t="n">
-        <v>0.51165119</v>
+        <v>0.42085373</v>
       </c>
       <c r="K37" s="7" t="n">
-        <v>77.0</v>
+        <v>85.0</v>
       </c>
       <c r="L37" s="7" t="n">
-        <v>6.79324675</v>
+        <v>5.03882353</v>
       </c>
       <c r="M37" s="7" t="n">
-        <v>4.0</v>
+        <v>11.0</v>
       </c>
       <c r="N37" s="7" t="n">
-        <v>130.77</v>
+        <v>38.93636364</v>
       </c>
       <c r="O37" s="7" t="n">
         <v>1.0</v>
       </c>
       <c r="P37" s="7" t="n">
-        <v>523.08</v>
+        <v>428.3</v>
       </c>
       <c r="Q37" s="7" t="n">
-        <v>2780.43</v>
+        <v>1970.51</v>
       </c>
       <c r="R37" s="7" t="n">
-        <v>5.31549667</v>
+        <v>4.60077049</v>
       </c>
       <c r="S37" s="8" t="s">
         <v>56</v>
@@ -2866,55 +2878,55 @@
         <v>57</v>
       </c>
       <c r="B38" s="5" t="n">
-        <v>482.56</v>
+        <v>422.78</v>
       </c>
       <c r="C38" s="6" t="n">
-        <v>16450.0</v>
+        <v>21954.0</v>
       </c>
       <c r="D38" s="7" t="n">
-        <v>29.33495441</v>
+        <v>19.25753849</v>
       </c>
       <c r="E38" s="6" t="n">
-        <v>9275.0</v>
+        <v>11094.0</v>
       </c>
       <c r="F38" s="7" t="n">
-        <v>52.02803235</v>
+        <v>38.10888769</v>
       </c>
       <c r="G38" s="7" t="n">
-        <v>1.77358491</v>
+        <v>1.97890752</v>
       </c>
       <c r="H38" s="7" t="n">
-        <v>73.0</v>
+        <v>75.0</v>
       </c>
       <c r="I38" s="7" t="n">
-        <v>6.61041096</v>
+        <v>5.63706667</v>
       </c>
       <c r="J38" s="7" t="n">
-        <v>0.443769</v>
+        <v>0.34162339</v>
       </c>
       <c r="K38" s="7" t="n">
-        <v>64.0</v>
+        <v>71.0</v>
       </c>
       <c r="L38" s="7" t="n">
-        <v>7.54</v>
+        <v>5.95464789</v>
       </c>
       <c r="M38" s="7" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="N38" s="7" t="n">
-        <v>241.28</v>
+        <v>42.278</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="P38" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Q38" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="R38" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S38" s="8" t="s">
         <v>57</v>
@@ -2928,55 +2940,55 @@
         <v>58</v>
       </c>
       <c r="B39" s="5" t="n">
-        <v>490.06</v>
+        <v>499.52</v>
       </c>
       <c r="C39" s="6" t="n">
-        <v>18558.0</v>
+        <v>22339.0</v>
       </c>
       <c r="D39" s="7" t="n">
-        <v>26.4069404</v>
+        <v>22.3608935</v>
       </c>
       <c r="E39" s="6" t="n">
-        <v>10573.0</v>
+        <v>11535.0</v>
       </c>
       <c r="F39" s="7" t="n">
-        <v>46.35013714</v>
+        <v>43.30472475</v>
       </c>
       <c r="G39" s="7" t="n">
-        <v>1.75522557</v>
+        <v>1.93662765</v>
       </c>
       <c r="H39" s="7" t="n">
-        <v>78.0</v>
+        <v>110.0</v>
       </c>
       <c r="I39" s="7" t="n">
-        <v>6.28282051</v>
+        <v>4.54109091</v>
       </c>
       <c r="J39" s="7" t="n">
-        <v>0.42030391</v>
+        <v>0.49241237</v>
       </c>
       <c r="K39" s="7" t="n">
-        <v>64.0</v>
+        <v>92.0</v>
       </c>
       <c r="L39" s="7" t="n">
-        <v>7.6571875</v>
+        <v>5.42956522</v>
       </c>
       <c r="M39" s="7" t="n">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="N39" s="7" t="n">
-        <v>49.006</v>
-      </c>
-      <c r="O39" s="7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="P39" s="7" t="n">
-        <v>163.35333333</v>
-      </c>
-      <c r="Q39" s="7" t="n">
-        <v>4661.42</v>
-      </c>
-      <c r="R39" s="7" t="n">
-        <v>9.51193731</v>
+        <v>62.44</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="S39" s="8" t="s">
         <v>58</v>
@@ -2990,55 +3002,55 @@
         <v>59</v>
       </c>
       <c r="B40" s="5" t="n">
-        <v>479.09</v>
+        <v>517.29</v>
       </c>
       <c r="C40" s="6" t="n">
-        <v>23706.0</v>
+        <v>20548.0</v>
       </c>
       <c r="D40" s="7" t="n">
-        <v>20.20965157</v>
+        <v>25.17471287</v>
       </c>
       <c r="E40" s="6" t="n">
-        <v>13139.0</v>
+        <v>9854.0</v>
       </c>
       <c r="F40" s="7" t="n">
-        <v>36.46320116</v>
+        <v>52.49543333</v>
       </c>
       <c r="G40" s="7" t="n">
-        <v>1.8042469</v>
+        <v>2.08524457</v>
       </c>
       <c r="H40" s="7" t="n">
-        <v>78.0</v>
+        <v>133.0</v>
       </c>
       <c r="I40" s="7" t="n">
-        <v>6.14217949</v>
+        <v>3.8893985</v>
       </c>
       <c r="J40" s="7" t="n">
-        <v>0.32903063</v>
+        <v>0.64726494</v>
       </c>
       <c r="K40" s="7" t="n">
-        <v>67.0</v>
+        <v>109.0</v>
       </c>
       <c r="L40" s="7" t="n">
-        <v>7.15059701</v>
+        <v>4.74577982</v>
       </c>
       <c r="M40" s="7" t="n">
-        <v>6.0</v>
+        <v>13.0</v>
       </c>
       <c r="N40" s="7" t="n">
-        <v>79.84833333</v>
+        <v>39.79153846</v>
       </c>
       <c r="O40" s="7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="P40" s="7" t="n">
-        <v>479.09</v>
+        <v>172.43</v>
       </c>
       <c r="Q40" s="7" t="n">
-        <v>1387.76</v>
+        <v>3008.3</v>
       </c>
       <c r="R40" s="7" t="n">
-        <v>2.89665825</v>
+        <v>5.81550001</v>
       </c>
       <c r="S40" s="8" t="s">
         <v>59</v>
@@ -3052,55 +3064,55 @@
         <v>60</v>
       </c>
       <c r="B41" s="5" t="n">
-        <v>478.54</v>
+        <v>523.08</v>
       </c>
       <c r="C41" s="6" t="n">
-        <v>23692.0</v>
+        <v>17981.0</v>
       </c>
       <c r="D41" s="7" t="n">
-        <v>20.1983792</v>
+        <v>29.09070686</v>
       </c>
       <c r="E41" s="6" t="n">
-        <v>11500.0</v>
+        <v>9592.0</v>
       </c>
       <c r="F41" s="7" t="n">
-        <v>41.61217391</v>
+        <v>54.53294412</v>
       </c>
       <c r="G41" s="7" t="n">
-        <v>2.06017391</v>
+        <v>1.87458299</v>
       </c>
       <c r="H41" s="7" t="n">
-        <v>83.0</v>
+        <v>92.0</v>
       </c>
       <c r="I41" s="7" t="n">
-        <v>5.76554217</v>
+        <v>5.68565217</v>
       </c>
       <c r="J41" s="7" t="n">
-        <v>0.35032923</v>
+        <v>0.51165119</v>
       </c>
       <c r="K41" s="7" t="n">
-        <v>68.0</v>
+        <v>77.0</v>
       </c>
       <c r="L41" s="7" t="n">
-        <v>7.03735294</v>
+        <v>6.79324675</v>
       </c>
       <c r="M41" s="7" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="N41" s="7" t="n">
-        <v>79.75666667</v>
-      </c>
-      <c r="O41" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P41" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q41" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R41" s="7" t="s">
-        <v>26</v>
+        <v>130.77</v>
+      </c>
+      <c r="O41" s="7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P41" s="7" t="n">
+        <v>523.08</v>
+      </c>
+      <c r="Q41" s="7" t="n">
+        <v>2780.43</v>
+      </c>
+      <c r="R41" s="7" t="n">
+        <v>5.31549667</v>
       </c>
       <c r="S41" s="8" t="s">
         <v>60</v>
@@ -3114,61 +3126,309 @@
         <v>61</v>
       </c>
       <c r="B42" s="5" t="n">
-        <v>383.72</v>
+        <v>482.56</v>
       </c>
       <c r="C42" s="6" t="n">
-        <v>19039.0</v>
+        <v>16450.0</v>
       </c>
       <c r="D42" s="7" t="n">
-        <v>20.15441987</v>
+        <v>29.33495441</v>
       </c>
       <c r="E42" s="6" t="n">
-        <v>10489.0</v>
+        <v>9275.0</v>
       </c>
       <c r="F42" s="7" t="n">
-        <v>36.58308704</v>
+        <v>52.02803235</v>
       </c>
       <c r="G42" s="7" t="n">
-        <v>1.81513967</v>
+        <v>1.77358491</v>
       </c>
       <c r="H42" s="7" t="n">
-        <v>63.0</v>
+        <v>73.0</v>
       </c>
       <c r="I42" s="7" t="n">
-        <v>6.09079365</v>
+        <v>6.61041096</v>
       </c>
       <c r="J42" s="7" t="n">
-        <v>0.33089973</v>
+        <v>0.443769</v>
       </c>
       <c r="K42" s="7" t="n">
-        <v>42.0</v>
+        <v>64.0</v>
       </c>
       <c r="L42" s="7" t="n">
-        <v>9.13619048</v>
+        <v>7.54</v>
       </c>
       <c r="M42" s="7" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="N42" s="7" t="n">
-        <v>54.81714286</v>
-      </c>
-      <c r="O42" s="7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="P42" s="7" t="n">
-        <v>191.86</v>
-      </c>
-      <c r="Q42" s="7" t="n">
-        <v>3241.14</v>
-      </c>
-      <c r="R42" s="7" t="n">
-        <v>8.44662775</v>
+        <v>241.28</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R42" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="S42" s="8" t="s">
         <v>61</v>
       </c>
       <c r="T42" s="8" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>490.06</v>
+      </c>
+      <c r="C43" s="6" t="n">
+        <v>18558.0</v>
+      </c>
+      <c r="D43" s="7" t="n">
+        <v>26.4069404</v>
+      </c>
+      <c r="E43" s="6" t="n">
+        <v>10573.0</v>
+      </c>
+      <c r="F43" s="7" t="n">
+        <v>46.35013714</v>
+      </c>
+      <c r="G43" s="7" t="n">
+        <v>1.75522557</v>
+      </c>
+      <c r="H43" s="7" t="n">
+        <v>78.0</v>
+      </c>
+      <c r="I43" s="7" t="n">
+        <v>6.28282051</v>
+      </c>
+      <c r="J43" s="7" t="n">
+        <v>0.42030391</v>
+      </c>
+      <c r="K43" s="7" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="L43" s="7" t="n">
+        <v>7.6571875</v>
+      </c>
+      <c r="M43" s="7" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="N43" s="7" t="n">
+        <v>49.006</v>
+      </c>
+      <c r="O43" s="7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P43" s="7" t="n">
+        <v>163.35333333</v>
+      </c>
+      <c r="Q43" s="7" t="n">
+        <v>4661.42</v>
+      </c>
+      <c r="R43" s="7" t="n">
+        <v>9.51193731</v>
+      </c>
+      <c r="S43" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="T43" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>479.09</v>
+      </c>
+      <c r="C44" s="6" t="n">
+        <v>23706.0</v>
+      </c>
+      <c r="D44" s="7" t="n">
+        <v>20.20965157</v>
+      </c>
+      <c r="E44" s="6" t="n">
+        <v>13139.0</v>
+      </c>
+      <c r="F44" s="7" t="n">
+        <v>36.46320116</v>
+      </c>
+      <c r="G44" s="7" t="n">
+        <v>1.8042469</v>
+      </c>
+      <c r="H44" s="7" t="n">
+        <v>78.0</v>
+      </c>
+      <c r="I44" s="7" t="n">
+        <v>6.14217949</v>
+      </c>
+      <c r="J44" s="7" t="n">
+        <v>0.32903063</v>
+      </c>
+      <c r="K44" s="7" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="L44" s="7" t="n">
+        <v>7.15059701</v>
+      </c>
+      <c r="M44" s="7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="N44" s="7" t="n">
+        <v>79.84833333</v>
+      </c>
+      <c r="O44" s="7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P44" s="7" t="n">
+        <v>479.09</v>
+      </c>
+      <c r="Q44" s="7" t="n">
+        <v>1387.76</v>
+      </c>
+      <c r="R44" s="7" t="n">
+        <v>2.89665825</v>
+      </c>
+      <c r="S44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T44" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>478.54</v>
+      </c>
+      <c r="C45" s="6" t="n">
+        <v>23692.0</v>
+      </c>
+      <c r="D45" s="7" t="n">
+        <v>20.1983792</v>
+      </c>
+      <c r="E45" s="6" t="n">
+        <v>11500.0</v>
+      </c>
+      <c r="F45" s="7" t="n">
+        <v>41.61217391</v>
+      </c>
+      <c r="G45" s="7" t="n">
+        <v>2.06017391</v>
+      </c>
+      <c r="H45" s="7" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="I45" s="7" t="n">
+        <v>5.76554217</v>
+      </c>
+      <c r="J45" s="7" t="n">
+        <v>0.35032923</v>
+      </c>
+      <c r="K45" s="7" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="L45" s="7" t="n">
+        <v>7.03735294</v>
+      </c>
+      <c r="M45" s="7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="N45" s="7" t="n">
+        <v>79.75666667</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="S45" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="T45" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="5" t="n">
+        <v>383.72</v>
+      </c>
+      <c r="C46" s="6" t="n">
+        <v>19039.0</v>
+      </c>
+      <c r="D46" s="7" t="n">
+        <v>20.15441987</v>
+      </c>
+      <c r="E46" s="6" t="n">
+        <v>10489.0</v>
+      </c>
+      <c r="F46" s="7" t="n">
+        <v>36.58308704</v>
+      </c>
+      <c r="G46" s="7" t="n">
+        <v>1.81513967</v>
+      </c>
+      <c r="H46" s="7" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="I46" s="7" t="n">
+        <v>6.09079365</v>
+      </c>
+      <c r="J46" s="7" t="n">
+        <v>0.33089973</v>
+      </c>
+      <c r="K46" s="7" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="L46" s="7" t="n">
+        <v>9.13619048</v>
+      </c>
+      <c r="M46" s="7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="N46" s="7" t="n">
+        <v>54.81714286</v>
+      </c>
+      <c r="O46" s="7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P46" s="7" t="n">
+        <v>191.86</v>
+      </c>
+      <c r="Q46" s="7" t="n">
+        <v>3241.14</v>
+      </c>
+      <c r="R46" s="7" t="n">
+        <v>8.44662775</v>
+      </c>
+      <c r="S46" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="T46" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>